<commit_message>
new conflict summary for events new wrong and right images TRUE/FALSE are now automatically converted to true/false BU02_template updated
</commit_message>
<xml_diff>
--- a/templates/BU02_template.xlsx
+++ b/templates/BU02_template.xlsx
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>GEN_First name_T</t>
   </si>
   <si>
     <t>GEN_PLACE_CountryOfResidence_T</t>
@@ -169,16 +166,10 @@
     <t>Treamtnent outcome</t>
   </si>
   <si>
-    <t>GEN_UID</t>
-  </si>
-  <si>
     <t>GEN_Age_atDiagnosis_T</t>
   </si>
   <si>
     <t>GEN_Sexe_T</t>
-  </si>
-  <si>
-    <t>Skin_Cl_Classification_T</t>
   </si>
   <si>
     <t>Skin_Cl_Lesion_Nodule_T</t>
@@ -226,19 +217,28 @@
     <t>Skin_Cl_Lesion_Loc_Upper limb_T</t>
   </si>
   <si>
-    <t>Skin_Cl_joint limitation_T</t>
-  </si>
-  <si>
     <t>Lab_Spe_YN_T</t>
   </si>
   <si>
     <t>BU_Lab_PCR_Initial Results_T</t>
   </si>
   <si>
-    <t>BU_Tx_AB_YNU_T</t>
+    <t>BU_Tx_AB_T</t>
   </si>
   <si>
-    <t>Skin_Cl_Lesion_Papule_T</t>
+    <t>DE_PR_GEN_UID</t>
+  </si>
+  <si>
+    <t>Skin_Cl_Papule_Lesion_T</t>
+  </si>
+  <si>
+    <t>GEN_FirstName_T</t>
+  </si>
+  <si>
+    <t>Skin_Cl_Classif_T</t>
+  </si>
+  <si>
+    <t>Skin_Cl_jointLimitation_T</t>
   </si>
 </sst>
 </file>
@@ -693,9 +693,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CY2566"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="AG9" sqref="AG9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +704,7 @@
     <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.140625" bestFit="1" customWidth="1"/>
@@ -745,130 +745,130 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>50</v>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>3</v>
+      <c r="M1" s="2" t="s">
+        <v>53</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="X1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:103" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:103" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:103" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:103" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="AA3"/>
       <c r="AB3"/>
@@ -948,100 +948,100 @@
     </row>
     <row r="4" spans="1:103" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="J4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="M4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="N4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="Q4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="S4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="S4" s="6" t="s">
+      <c r="T4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="U4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="U4" s="6" t="s">
+      <c r="V4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="W4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="W4" s="6" t="s">
+      <c r="X4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="X4" s="9" t="s">
+      <c r="Y4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="Y4" s="6" t="s">
+      <c r="Z4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="Z4" s="6" t="s">
+      <c r="AA4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AA4" s="6" t="s">
+      <c r="AB4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AB4" s="6" t="s">
+      <c r="AC4" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AC4" s="6" t="s">
+      <c r="AD4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE4" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="AD4" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE4" s="11" t="s">
-        <v>46</v>
-      </c>
       <c r="AF4" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AG4"/>
       <c r="AH4"/>
@@ -8637,5 +8637,6 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
2.13.0 tested template fixed
</commit_message>
<xml_diff>
--- a/templates/BU02_template.xlsx
+++ b/templates/BU02_template.xlsx
@@ -223,9 +223,6 @@
     <t>BU_Lab_PCR_Initial Results_T</t>
   </si>
   <si>
-    <t>BU_Tx_AB_T</t>
-  </si>
-  <si>
     <t>DE_PR_GEN_UID</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>Skin_Cl_jointLimitation_T</t>
+  </si>
+  <si>
+    <t>BU_Tx_AB_YNU_T</t>
   </si>
 </sst>
 </file>
@@ -695,7 +695,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG9" sqref="AG9"/>
+      <selection pane="bottomLeft" activeCell="AF20" sqref="AF20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,10 +745,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>49</v>
@@ -763,7 +763,7 @@
         <v>3</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>51</v>
@@ -775,7 +775,7 @@
         <v>53</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>54</v>
@@ -817,7 +817,7 @@
         <v>4</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AC1" s="2" t="s">
         <v>66</v>
@@ -826,7 +826,7 @@
         <v>67</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AF1" s="2" t="s">
         <v>47</v>

</xml_diff>